<commit_message>
Incluir archivos ECS faltantes segun el PGS
</commit_message>
<xml_diff>
--- a/Biblioteca de Trabajo/1. ELICITACION/1.3 Matriz IREB/G4_27835_Matriz_IREBv1.0.xlsx
+++ b/Biblioteca de Trabajo/1. ELICITACION/1.3 Matriz IREB/G4_27835_Matriz_IREBv1.0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29415"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6910969B-A2AA-4464-848E-56D361429694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC579A44-3D08-429A-8D31-B40B6AE7F9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,8 +13,7 @@
     <sheet name="RF8" sheetId="10" r:id="rId3"/>
     <sheet name="RF11.2" sheetId="3" r:id="rId4"/>
     <sheet name="Recomend RF13" sheetId="11" r:id="rId5"/>
-    <sheet name="Recomend RF8" sheetId="12" r:id="rId6"/>
-    <sheet name="Recomend RF11.2" sheetId="5" r:id="rId7"/>
+    <sheet name="Recomend RF11.2" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -757,7 +756,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="103">
   <si>
     <t>MATRIZ PARA COMPROBACIÓN REQUERIMIENTOS DE CALIDAD DE PROYECTO ACADEMICO</t>
   </si>
@@ -893,7 +892,7 @@
   </si>
   <si>
     <t xml:space="preserve">
-1. No ha sido desarrollado, sea a utilizado un prototipo usable de manera solo visual.</t>
+1. La visualizacion se ha desarrollado para su uso.</t>
   </si>
   <si>
     <t>1. No ha sido desarrollado un prototipo usable solo de manera visual.
@@ -1075,18 +1074,6 @@
   </si>
   <si>
     <t>Generar una tabla de términos complejos o no tan entendibles para los interesados para que, llegado el caso de leer el documento, puedan informarse correctamente sobre la labor de cada función especificada.</t>
-  </si>
-  <si>
-    <t>¿Se ha incorporado los cambios sugeridos por el cliente?</t>
-  </si>
-  <si>
-    <t>Se recomienda establecer un proceso formal de gestión de cambios que incluya el registro, revisión e incorporación de cada sugerencia recibida por parte del cliente, asegurando que los requisitos estén actualizados, reflejen las expectativas reales y requeridas por el cliente para asi evitar malos entendiendos.</t>
-  </si>
-  <si>
-    <t>¿El requerimiento especifica cómo se visualizará el progreso o solo indica que se mostrará sin detallar su funcionamiento?</t>
-  </si>
-  <si>
-    <t>Se podria detallar claramente cómo se implementará la visualización del progreso. Especifica qué datos se mostrarán ,y cómo el usuario podrá verificar su historial. Esto garantiza que el requerimiento sea realizable, verificable y útil.</t>
   </si>
   <si>
     <t>¿Es verificable y se puede compobar con un esfuerzo razonable?</t>
@@ -1418,7 +1405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1496,11 +1483,47 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1520,11 +1543,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="15" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1535,49 +1563,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1585,6 +1573,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
@@ -3165,8 +3156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E34895F-ADFF-4BB8-A97F-5DAA9AAD6C3C}">
   <dimension ref="B1:K1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3192,107 +3183,107 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="2:11" ht="30" customHeight="1">
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
     </row>
     <row r="4" spans="2:11" ht="30" customHeight="1">
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
     </row>
     <row r="5" spans="2:11" ht="30" customHeight="1">
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
     </row>
     <row r="6" spans="2:11" ht="55.5" customHeight="1">
       <c r="C6" s="1"/>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="59"/>
     </row>
     <row r="7" spans="2:11" ht="45" customHeight="1">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="59"/>
-      <c r="E7" s="46" t="s">
+      <c r="D7" s="60"/>
+      <c r="E7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="46" t="s">
+      <c r="G7" s="29" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="4">
         <v>100</v>
       </c>
-      <c r="I7" s="44" t="s">
+      <c r="I7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="46" t="s">
+      <c r="J7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="44" t="s">
+      <c r="K7" s="30" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="60" customHeight="1">
-      <c r="B8" s="60"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="60"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="61"/>
       <c r="H8" s="4">
         <v>0</v>
       </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
     </row>
     <row r="9" spans="2:11" ht="48.75">
       <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="58"/>
+      <c r="D9" s="59"/>
       <c r="E9" s="6" t="s">
         <v>11</v>
       </c>
@@ -3319,10 +3310,10 @@
       <c r="B10" s="5">
         <v>2</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="58"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="6" t="s">
         <v>11</v>
       </c>
@@ -3346,10 +3337,10 @@
       <c r="B11" s="5">
         <v>3</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="58"/>
+      <c r="D11" s="59"/>
       <c r="E11" s="6" t="s">
         <v>11</v>
       </c>
@@ -3373,10 +3364,10 @@
       <c r="B12" s="5">
         <v>4</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="58"/>
+      <c r="D12" s="59"/>
       <c r="E12" s="6" t="s">
         <v>11</v>
       </c>
@@ -3389,21 +3380,21 @@
       <c r="I12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="30" t="s">
+      <c r="J12" s="41" t="s">
         <v>11</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="87" customHeight="1">
+    <row r="13" spans="2:11" ht="64.5">
       <c r="B13" s="5">
         <v>5</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="58"/>
+      <c r="D13" s="59"/>
       <c r="E13" s="6" t="s">
         <v>11</v>
       </c>
@@ -3427,11 +3418,11 @@
       <c r="B14" s="5">
         <v>6</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="29" t="s">
+      <c r="D14" s="59"/>
+      <c r="E14" s="40" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="10" t="s">
@@ -3443,7 +3434,7 @@
       <c r="I14" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="30" t="s">
+      <c r="J14" s="41" t="s">
         <v>11</v>
       </c>
       <c r="K14" s="10" t="s">
@@ -3454,17 +3445,17 @@
       <c r="B15" s="5">
         <v>7</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="30" t="s">
+      <c r="D15" s="59"/>
+      <c r="E15" s="41" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="41" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="10" t="s">
@@ -3481,18 +3472,18 @@
       <c r="B16" s="5">
         <v>8</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="58"/>
-      <c r="E16" s="30" t="s">
+      <c r="D16" s="59"/>
+      <c r="E16" s="41" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>24</v>
+      <c r="G16" s="41" t="s">
+        <v>11</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>41</v>
@@ -3508,10 +3499,10 @@
       <c r="B17" s="5">
         <v>9</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="58"/>
+      <c r="D17" s="59"/>
       <c r="E17" s="6" t="s">
         <v>11</v>
       </c>
@@ -3524,7 +3515,7 @@
       <c r="I17" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="J17" s="30" t="s">
+      <c r="J17" s="41" t="s">
         <v>11</v>
       </c>
       <c r="K17" s="12" t="s">
@@ -3535,10 +3526,10 @@
       <c r="B18" s="5">
         <v>10</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="58"/>
+      <c r="D18" s="59"/>
       <c r="E18" s="6" t="s">
         <v>11</v>
       </c>
@@ -3562,23 +3553,23 @@
       <c r="B19" s="5">
         <v>11</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="29" t="s">
+      <c r="D19" s="59"/>
+      <c r="E19" s="40" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="G19" s="40" t="s">
         <v>24</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J19" s="29" t="s">
+      <c r="J19" s="40" t="s">
         <v>24</v>
       </c>
       <c r="K19" s="10" t="s">
@@ -6530,6 +6521,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="C9:D9"/>
@@ -6537,11 +6533,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C3:K4"/>
     <mergeCell ref="E5:K5"/>
     <mergeCell ref="F6:K6"/>
@@ -6584,15 +6575,15 @@
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
       <c r="J1" s="13"/>
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
@@ -6615,37 +6606,37 @@
       <c r="B2" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="53">
+      <c r="C2" s="37">
         <v>45946</v>
       </c>
-      <c r="D2" s="56"/>
+      <c r="D2" s="49"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="B3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="49"/>
     </row>
     <row r="4" spans="1:26" ht="18.75">
       <c r="B4" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="16" t="s">
@@ -6662,7 +6653,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="30.75">
-      <c r="A8" s="31">
+      <c r="A8" s="43">
         <v>1</v>
       </c>
       <c r="B8" s="19" t="s">
@@ -6671,10 +6662,10 @@
       <c r="C8" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="44"/>
     </row>
     <row r="9" spans="1:26" ht="30.75">
-      <c r="A9" s="31">
+      <c r="A9" s="43">
         <v>2</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -6683,10 +6674,10 @@
       <c r="C9" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="44"/>
     </row>
     <row r="10" spans="1:26" ht="60.75">
-      <c r="A10" s="31">
+      <c r="A10" s="43">
         <v>3</v>
       </c>
       <c r="B10" s="19" t="s">
@@ -6695,10 +6686,10 @@
       <c r="C10" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="32"/>
+      <c r="D10" s="44"/>
     </row>
     <row r="11" spans="1:26" ht="30.75">
-      <c r="A11" s="31">
+      <c r="A11" s="43">
         <v>4</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -6707,10 +6698,10 @@
       <c r="C11" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:26" ht="30.75">
-      <c r="A12" s="31">
+      <c r="A12" s="43">
         <v>5</v>
       </c>
       <c r="B12" s="19" t="s">
@@ -6719,10 +6710,10 @@
       <c r="C12" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="32"/>
+      <c r="D12" s="44"/>
     </row>
     <row r="13" spans="1:26" ht="30.75">
-      <c r="A13" s="31">
+      <c r="A13" s="43">
         <v>6</v>
       </c>
       <c r="B13" s="19" t="s">
@@ -6731,22 +6722,22 @@
       <c r="C13" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="32"/>
+      <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:26" ht="30.75">
-      <c r="A14" s="31">
+      <c r="A14" s="43">
         <v>7</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>70</v>
       </c>
       <c r="C14" s="20"/>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="44" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="45.75">
-      <c r="A15" s="31">
+      <c r="A15" s="43">
         <v>8</v>
       </c>
       <c r="B15" s="19" t="s">
@@ -6755,7 +6746,7 @@
       <c r="C15" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" s="44"/>
     </row>
     <row r="16" spans="1:26" ht="60.75">
       <c r="A16" s="21">
@@ -6770,10 +6761,10 @@
       <c r="D16" s="23"/>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="25">
         <f>COUNTA('RF13'!$C$8:$C$16)</f>
         <v>8</v>
@@ -6784,10 +6775,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="56"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="26">
         <f t="shared" ref="C18:D18" si="0">C17/9</f>
         <v>0.88888888888888884</v>
@@ -6804,29 +6795,29 @@
       <c r="D19" s="25"/>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="48" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30.75">
-      <c r="A22" s="31">
+      <c r="A22" s="43">
         <v>1</v>
       </c>
       <c r="B22" s="19" t="s">
@@ -6835,10 +6826,10 @@
       <c r="C22" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="32"/>
+      <c r="D22" s="44"/>
     </row>
     <row r="23" spans="1:4" ht="30.75">
-      <c r="A23" s="31">
+      <c r="A23" s="43">
         <v>2</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -6847,10 +6838,10 @@
       <c r="C23" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="44"/>
     </row>
     <row r="24" spans="1:4" ht="30.75">
-      <c r="A24" s="31">
+      <c r="A24" s="43">
         <v>3</v>
       </c>
       <c r="B24" s="19" t="s">
@@ -6859,10 +6850,10 @@
       <c r="C24" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="44"/>
     </row>
     <row r="25" spans="1:4" ht="30.75">
-      <c r="A25" s="31">
+      <c r="A25" s="43">
         <v>4</v>
       </c>
       <c r="B25" s="19" t="s">
@@ -6871,7 +6862,7 @@
       <c r="C25" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="44"/>
     </row>
     <row r="26" spans="1:4" ht="30.75">
       <c r="A26" s="21">
@@ -6886,10 +6877,10 @@
       <c r="D26" s="27"/>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="56"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="25">
         <f>COUNTA('RF13'!$C$22:$C$26)</f>
         <v>5</v>
@@ -6900,10 +6891,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="56"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="26">
         <f t="shared" ref="C28:D28" si="1">C27/5</f>
         <v>1</v>
@@ -6920,29 +6911,29 @@
       <c r="D29" s="25"/>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="48" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30.75">
-      <c r="A32" s="31">
+      <c r="A32" s="43">
         <v>1</v>
       </c>
       <c r="B32" s="19" t="s">
@@ -6954,7 +6945,7 @@
       <c r="D32" s="23"/>
     </row>
     <row r="33" spans="1:4" ht="45.75">
-      <c r="A33" s="31">
+      <c r="A33" s="43">
         <v>2</v>
       </c>
       <c r="B33" s="19" t="s">
@@ -6978,10 +6969,10 @@
       <c r="D34" s="23"/>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A35" s="50" t="s">
+      <c r="A35" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="56"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="8">
         <f>COUNTA('RF13'!$C$32:$C$34)</f>
         <v>3</v>
@@ -6992,10 +6983,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="56"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="26">
         <f t="shared" ref="C36:D36" si="2">C35/3</f>
         <v>1</v>
@@ -7009,11 +7000,11 @@
     <row r="38" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A40" s="52" t="s">
+      <c r="A40" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
     </row>
     <row r="41" spans="1:4" ht="30" customHeight="1">
       <c r="B41" s="13" t="s">
@@ -8010,12 +8001,12 @@
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A35:B35"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <conditionalFormatting sqref="A32:D34">
     <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="X">
@@ -8090,15 +8081,15 @@
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
       <c r="J1" s="13"/>
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
@@ -8121,37 +8112,37 @@
       <c r="B2" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="53">
+      <c r="C2" s="37">
         <v>45946</v>
       </c>
-      <c r="D2" s="56"/>
+      <c r="D2" s="49"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="B3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="49"/>
     </row>
     <row r="4" spans="1:26" ht="18.75">
       <c r="B4" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="16" t="s">
@@ -8168,7 +8159,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="31">
+      <c r="A8" s="43">
         <v>1</v>
       </c>
       <c r="B8" s="19" t="s">
@@ -8177,10 +8168,10 @@
       <c r="C8" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="44"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="31">
+      <c r="A9" s="43">
         <v>2</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -8189,10 +8180,10 @@
       <c r="C9" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="44"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="31">
+      <c r="A10" s="43">
         <v>3</v>
       </c>
       <c r="B10" s="19" t="s">
@@ -8201,10 +8192,10 @@
       <c r="C10" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="32"/>
+      <c r="D10" s="44"/>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="31">
+      <c r="A11" s="43">
         <v>4</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -8213,10 +8204,10 @@
       <c r="C11" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="31">
+      <c r="A12" s="43">
         <v>5</v>
       </c>
       <c r="B12" s="19" t="s">
@@ -8225,10 +8216,10 @@
       <c r="C12" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="32"/>
+      <c r="D12" s="44"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="31">
+      <c r="A13" s="43">
         <v>6</v>
       </c>
       <c r="B13" s="19" t="s">
@@ -8237,10 +8228,10 @@
       <c r="C13" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="32"/>
+      <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="31">
+      <c r="A14" s="43">
         <v>7</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -8249,10 +8240,10 @@
       <c r="C14" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="32"/>
+      <c r="D14" s="44"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="31">
+      <c r="A15" s="43">
         <v>8</v>
       </c>
       <c r="B15" s="19" t="s">
@@ -8261,7 +8252,7 @@
       <c r="C15" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" s="44"/>
     </row>
     <row r="16" spans="1:26" ht="60.75">
       <c r="A16" s="21">
@@ -8276,10 +8267,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="25">
         <f>COUNTA('RF8'!$C$8:$C$16)</f>
         <v>8</v>
@@ -8290,10 +8281,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="56"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="26">
         <f>C17/9</f>
         <v>0.88888888888888884</v>
@@ -8310,29 +8301,29 @@
       <c r="D19" s="25"/>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="48" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A22" s="31">
+      <c r="A22" s="43">
         <v>1</v>
       </c>
       <c r="B22" s="19" t="s">
@@ -8341,10 +8332,10 @@
       <c r="C22" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="32"/>
+      <c r="D22" s="44"/>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A23" s="31">
+      <c r="A23" s="43">
         <v>2</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -8353,10 +8344,10 @@
       <c r="C23" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="44"/>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A24" s="31">
+      <c r="A24" s="43">
         <v>3</v>
       </c>
       <c r="B24" s="19" t="s">
@@ -8365,10 +8356,10 @@
       <c r="C24" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="44"/>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A25" s="31">
+      <c r="A25" s="43">
         <v>4</v>
       </c>
       <c r="B25" s="19" t="s">
@@ -8377,7 +8368,7 @@
       <c r="C25" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="44"/>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" s="21">
@@ -8392,10 +8383,10 @@
       <c r="D26" s="27"/>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="56"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="25">
         <f>COUNTA('RF8'!$C$22:$C$26)</f>
         <v>5</v>
@@ -8406,10 +8397,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="56"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="26">
         <f>C27/5</f>
         <v>1</v>
@@ -8426,29 +8417,29 @@
       <c r="D29" s="25"/>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="48" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A32" s="31">
+      <c r="A32" s="43">
         <v>1</v>
       </c>
       <c r="B32" s="19" t="s">
@@ -8460,7 +8451,7 @@
       <c r="D32" s="23"/>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A33" s="31">
+      <c r="A33" s="43">
         <v>2</v>
       </c>
       <c r="B33" s="19" t="s">
@@ -8484,10 +8475,10 @@
       <c r="D34" s="23"/>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A35" s="50" t="s">
+      <c r="A35" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="56"/>
+      <c r="B35" s="49"/>
       <c r="C35">
         <f>COUNTA('RF8'!$C$32:$C$34)</f>
         <v>3</v>
@@ -8498,10 +8489,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="56"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="26">
         <f>C35/3</f>
         <v>1</v>
@@ -8515,11 +8506,11 @@
     <row r="38" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A40" s="52" t="s">
+      <c r="A40" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
     </row>
     <row r="41" spans="1:4" ht="30" customHeight="1">
       <c r="B41" s="13" t="s">
@@ -9516,12 +9507,12 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A17:B17"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <conditionalFormatting sqref="A32:D34">
     <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="X">
@@ -9579,7 +9570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
@@ -9597,9 +9588,10 @@
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="50" t="s">
         <v>89</v>
       </c>
+      <c r="D1" s="51"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -9627,36 +9619,37 @@
       <c r="B2" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="52">
         <v>45946</v>
       </c>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="B3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="49"/>
     </row>
     <row r="4" spans="1:26" ht="18.75">
       <c r="B4" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="16" t="s">
@@ -9673,19 +9666,19 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="30.75">
-      <c r="A8" s="31">
+      <c r="A8" s="43">
         <v>1</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>63</v>
       </c>
       <c r="C8" s="20"/>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="44" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="30.75">
-      <c r="A9" s="31">
+      <c r="A9" s="43">
         <v>2</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -9694,10 +9687,10 @@
       <c r="C9" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="44"/>
     </row>
     <row r="10" spans="1:26" ht="60.75">
-      <c r="A10" s="31">
+      <c r="A10" s="43">
         <v>3</v>
       </c>
       <c r="B10" s="19" t="s">
@@ -9706,10 +9699,10 @@
       <c r="C10" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="32"/>
+      <c r="D10" s="44"/>
     </row>
     <row r="11" spans="1:26" ht="30.75">
-      <c r="A11" s="31">
+      <c r="A11" s="43">
         <v>4</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -9718,10 +9711,10 @@
       <c r="C11" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:26" ht="30.75">
-      <c r="A12" s="31">
+      <c r="A12" s="43">
         <v>5</v>
       </c>
       <c r="B12" s="19" t="s">
@@ -9730,10 +9723,10 @@
       <c r="C12" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="32"/>
+      <c r="D12" s="44"/>
     </row>
     <row r="13" spans="1:26" ht="30.75">
-      <c r="A13" s="31">
+      <c r="A13" s="43">
         <v>6</v>
       </c>
       <c r="B13" s="19" t="s">
@@ -9742,10 +9735,10 @@
       <c r="C13" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="32"/>
+      <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:26" ht="30.75">
-      <c r="A14" s="31">
+      <c r="A14" s="43">
         <v>7</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -9754,10 +9747,10 @@
       <c r="C14" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="20"/>
+      <c r="D14" s="53"/>
     </row>
     <row r="15" spans="1:26" ht="45.75">
-      <c r="A15" s="31">
+      <c r="A15" s="43">
         <v>8</v>
       </c>
       <c r="B15" s="19" t="s">
@@ -9766,7 +9759,7 @@
       <c r="C15" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" s="44"/>
     </row>
     <row r="16" spans="1:26" ht="60.75">
       <c r="A16" s="21">
@@ -9781,10 +9774,10 @@
       <c r="D16" s="23"/>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="25">
         <f>COUNTA('RF11.2'!$C$8:$C$16)</f>
         <v>8</v>
@@ -9795,16 +9788,16 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="56"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="26">
         <f t="shared" ref="C18:D18" si="0">C17/9</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="D18" s="26">
-        <f>D17/9</f>
+        <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
@@ -9815,29 +9808,29 @@
       <c r="D19" s="25"/>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="48" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30.75">
-      <c r="A22" s="31">
+      <c r="A22" s="43">
         <v>1</v>
       </c>
       <c r="B22" s="19" t="s">
@@ -9846,10 +9839,10 @@
       <c r="C22" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="32"/>
+      <c r="D22" s="44"/>
     </row>
     <row r="23" spans="1:4" ht="30.75">
-      <c r="A23" s="31">
+      <c r="A23" s="43">
         <v>2</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -9858,22 +9851,22 @@
       <c r="C23" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="44"/>
     </row>
     <row r="24" spans="1:4" ht="30.75">
-      <c r="A24" s="31">
+      <c r="A24" s="43">
         <v>3</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>78</v>
       </c>
       <c r="C24" s="23"/>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="54" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30.75">
-      <c r="A25" s="31">
+      <c r="A25" s="43">
         <v>4</v>
       </c>
       <c r="B25" s="19" t="s">
@@ -9882,7 +9875,7 @@
       <c r="C25" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="44"/>
     </row>
     <row r="26" spans="1:4" ht="30.75">
       <c r="A26" s="21">
@@ -9897,10 +9890,10 @@
       <c r="D26" s="27"/>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="56"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="25">
         <f>COUNTA('RF11.2'!$C$22:$C$26)</f>
         <v>4</v>
@@ -9911,10 +9904,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="56"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="26">
         <f t="shared" ref="C28:D28" si="1">C27/5</f>
         <v>0.8</v>
@@ -9931,47 +9924,47 @@
       <c r="D29" s="25"/>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="48" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30.75">
-      <c r="A32" s="31">
+      <c r="A32" s="43">
         <v>1</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="56" t="s">
         <v>64</v>
       </c>
       <c r="D32" s="23"/>
     </row>
     <row r="33" spans="1:4" ht="45.75">
-      <c r="A33" s="31">
+      <c r="A33" s="43">
         <v>2</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="40"/>
+      <c r="C33" s="55"/>
       <c r="D33" s="23" t="s">
         <v>64</v>
       </c>
@@ -9989,10 +9982,10 @@
       <c r="D34" s="23"/>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A35" s="50" t="s">
+      <c r="A35" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="56"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="8">
         <f>COUNTA('RF11.2'!$C$32:$C$34)</f>
         <v>2</v>
@@ -10003,10 +9996,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="56"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="26">
         <f t="shared" ref="C36:D36" si="2">C35/3</f>
         <v>0.66666666666666663</v>
@@ -10020,11 +10013,11 @@
     <row r="38" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A40" s="52" t="s">
+      <c r="A40" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
     </row>
     <row r="41" spans="1:4" ht="30" customHeight="1">
       <c r="B41" s="13" t="s">
@@ -12119,1050 +12112,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033E88DB-FE5E-4FE0-9EBF-6D3D816F6F84}">
-  <dimension ref="A1:B998"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1"/>
-    <col min="2" max="2" width="57.28515625" customWidth="1"/>
-    <col min="3" max="26" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A1" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="76.5">
-      <c r="A2" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60.75">
-      <c r="A3" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -13183,18 +12136,18 @@
     </row>
     <row r="2" spans="1:2" ht="45.75">
       <c r="A2" s="19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30.75">
       <c r="A3" s="19" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>